<commit_message>
22 cities of switzerland
expanded distance based cravity model to the 22 cities.
I have no idea why it doesn't work with gephi....
</commit_message>
<xml_diff>
--- a/code/A (first) Gravity Model/Gephi/data_for_gephi.xlsx
+++ b/code/A (first) Gravity Model/Gephi/data_for_gephi.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="150" windowWidth="14115" windowHeight="4395"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="data_for_gephi" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Zuerich</t>
   </si>
@@ -48,10 +48,70 @@
     <t>Biel</t>
   </si>
   <si>
-    <t>Olten</t>
-  </si>
-  <si>
-    <t>Arthgoldau</t>
+    <t xml:space="preserve">    Zuerich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Genf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Basel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lausanne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Bern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Winterthur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Luzern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    St.Gallen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lugano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Biel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Thun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Koeniz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    La Chaux-de-Fonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Schaffhausen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Freiburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Chur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Neuenburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Vernier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Uster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Olten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Arthgoldau</t>
   </si>
 </sst>
 </file>
@@ -383,15 +443,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:23">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -423,56 +491,116 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.1103999999999998</v>
+        <v>0.311</v>
       </c>
       <c r="D2">
-        <v>8.2011000000000003</v>
+        <v>0.82010000000000005</v>
       </c>
       <c r="E2">
-        <v>2.7387999999999999</v>
+        <v>0.27389999999999998</v>
       </c>
       <c r="F2">
-        <v>4.8220999999999998</v>
+        <v>0.48220000000000002</v>
       </c>
       <c r="G2">
         <v>1.8227</v>
       </c>
       <c r="H2">
-        <v>7.0673000000000004</v>
+        <v>0.70669999999999999</v>
       </c>
       <c r="I2">
-        <v>4.2964000000000002</v>
+        <v>0.42959999999999998</v>
       </c>
       <c r="J2">
-        <v>1.3105</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="K2">
-        <v>1.8802000000000001</v>
+        <v>0.188</v>
       </c>
       <c r="L2">
-        <v>9.1585999999999999</v>
+        <v>0.16270000000000001</v>
       </c>
       <c r="M2">
-        <v>1.1207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="N2">
+        <v>0.1047</v>
+      </c>
+      <c r="O2">
+        <v>0.35830000000000001</v>
+      </c>
+      <c r="P2">
+        <v>0.1062</v>
+      </c>
+      <c r="Q2">
+        <v>0.13170000000000001</v>
+      </c>
+      <c r="R2">
+        <v>9.5200000000000007E-2</v>
+      </c>
+      <c r="S2">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="T2">
+        <v>0.86829999999999996</v>
+      </c>
+      <c r="U2">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="V2">
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="W2">
+        <v>0.11210000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0.311</v>
@@ -481,133 +609,223 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.6388</v>
+        <v>0.16389999999999999</v>
       </c>
       <c r="E3">
-        <v>4.6787999999999998</v>
+        <v>0.46789999999999998</v>
       </c>
       <c r="F3">
-        <v>1.8028</v>
+        <v>0.18029999999999999</v>
       </c>
       <c r="G3">
         <v>7.7399999999999997E-2</v>
       </c>
       <c r="H3">
-        <v>0.76519999999999999</v>
+        <v>7.6499999999999999E-2</v>
       </c>
       <c r="I3">
-        <v>0.48620000000000002</v>
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="J3">
-        <v>0.46910000000000002</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="K3">
-        <v>0.71719999999999995</v>
+        <v>7.17E-2</v>
       </c>
       <c r="L3">
-        <v>1.1887000000000001</v>
+        <v>6.1699999999999998E-2</v>
       </c>
       <c r="M3">
-        <v>0.1004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="N3">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="O3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="P3">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="Q3">
+        <v>2.35E-2</v>
+      </c>
+      <c r="R3">
+        <v>5.8299999999999998E-2</v>
+      </c>
+      <c r="S3">
+        <v>1.5952999999999999</v>
+      </c>
+      <c r="T3">
+        <v>2.58E-2</v>
+      </c>
+      <c r="U3">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="V3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="W3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>0.82010000000000005</v>
       </c>
       <c r="C4">
-        <v>1.6388</v>
+        <v>0.16389999999999999</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.5255000000000001</v>
+        <v>0.15260000000000001</v>
       </c>
       <c r="F4">
-        <v>2.9674999999999998</v>
+        <v>0.29670000000000002</v>
       </c>
       <c r="G4">
         <v>0.18920000000000001</v>
       </c>
       <c r="H4">
-        <v>1.6268</v>
+        <v>0.16270000000000001</v>
       </c>
       <c r="I4">
-        <v>0.88</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="J4">
-        <v>0.44319999999999998</v>
+        <v>4.4299999999999999E-2</v>
       </c>
       <c r="K4">
-        <v>1.5625</v>
+        <v>0.15629999999999999</v>
       </c>
       <c r="L4">
-        <v>5.8457999999999997</v>
+        <v>7.8299999999999995E-2</v>
       </c>
       <c r="M4">
-        <v>0.19639999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="N4">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="O4">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="P4">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="Q4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="R4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="S4">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="T4">
+        <v>5.9799999999999999E-2</v>
+      </c>
+      <c r="U4">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="V4">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="W4">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0.27389999999999998</v>
       </c>
       <c r="C5">
-        <v>4.6787999999999998</v>
+        <v>0.46789999999999998</v>
       </c>
       <c r="D5">
-        <v>1.5255000000000001</v>
+        <v>0.15260000000000001</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2.0320999999999998</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="G5">
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="H5">
-        <v>0.70550000000000002</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="I5">
-        <v>0.4022</v>
+        <v>4.02E-2</v>
       </c>
       <c r="J5">
-        <v>0.37130000000000002</v>
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="K5">
-        <v>0.78459999999999996</v>
+        <v>7.85E-2</v>
       </c>
       <c r="L5">
-        <v>1.1192</v>
+        <v>6.7299999999999999E-2</v>
       </c>
       <c r="M5">
-        <v>8.9599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="N5">
+        <v>7.1900000000000006E-2</v>
+      </c>
+      <c r="O5">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="P5">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="Q5">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="R5">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="S5">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="T5">
+        <v>2.24E-2</v>
+      </c>
+      <c r="U5">
+        <v>6.0100000000000001E-2</v>
+      </c>
+      <c r="V5">
+        <v>1.12E-2</v>
+      </c>
+      <c r="W5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.48220000000000002</v>
       </c>
       <c r="C6">
-        <v>1.8028</v>
+        <v>0.18029999999999999</v>
       </c>
       <c r="D6">
-        <v>2.9674999999999998</v>
+        <v>0.29670000000000002</v>
       </c>
       <c r="E6">
-        <v>2.0320999999999998</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -616,83 +834,143 @@
         <v>0.1081</v>
       </c>
       <c r="H6">
-        <v>1.4510000000000001</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="I6">
-        <v>0.58160000000000001</v>
+        <v>5.8200000000000002E-2</v>
       </c>
       <c r="J6">
-        <v>0.43330000000000002</v>
+        <v>4.3299999999999998E-2</v>
       </c>
       <c r="K6">
-        <v>2.5154000000000001</v>
+        <v>0.2515</v>
       </c>
       <c r="L6">
-        <v>2.5617000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="M6">
-        <v>0.1615</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>1.4197</v>
+      </c>
+      <c r="N6">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="O6">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="P6">
+        <v>0.1638</v>
+      </c>
+      <c r="Q6">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="R6">
+        <v>0.1057</v>
+      </c>
+      <c r="S6">
+        <v>3.09E-2</v>
+      </c>
+      <c r="T6">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="U6">
+        <v>4.7199999999999999E-2</v>
+      </c>
+      <c r="V6">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="W6">
+        <v>1.6199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>1.8227</v>
       </c>
       <c r="C7">
-        <v>0.77410000000000001</v>
+        <v>7.7399999999999997E-2</v>
       </c>
       <c r="D7">
-        <v>1.8919999999999999</v>
+        <v>0.18920000000000001</v>
       </c>
       <c r="E7">
-        <v>0.66549999999999998</v>
+        <v>6.6600000000000006E-2</v>
       </c>
       <c r="F7">
-        <v>1.081</v>
+        <v>0.1081</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.2971999999999999</v>
+        <v>0.12970000000000001</v>
       </c>
       <c r="I7">
-        <v>1.5381</v>
+        <v>0.15379999999999999</v>
       </c>
       <c r="J7">
-        <v>0.33279999999999998</v>
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="K7">
-        <v>0.43030000000000002</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="L7">
-        <v>1.8174999999999999</v>
+        <v>3.6499999999999998E-2</v>
       </c>
       <c r="M7">
-        <v>0.2135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O7">
+        <v>0.14810000000000001</v>
+      </c>
+      <c r="P7">
+        <v>2.47E-2</v>
+      </c>
+      <c r="Q7">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="R7">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="S7">
+        <v>1.34E-2</v>
+      </c>
+      <c r="T7">
+        <v>0.19339999999999999</v>
+      </c>
+      <c r="U7">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="V7">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="W7">
+        <v>2.1399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0.70669999999999999</v>
       </c>
       <c r="C8">
-        <v>0.76519999999999999</v>
+        <v>7.6499999999999999E-2</v>
       </c>
       <c r="D8">
-        <v>1.6268</v>
+        <v>0.16270000000000001</v>
       </c>
       <c r="E8">
-        <v>0.70550000000000002</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="F8">
-        <v>1.4510000000000001</v>
+        <v>0.14510000000000001</v>
       </c>
       <c r="G8">
         <v>0.12970000000000001</v>
@@ -701,223 +979,1113 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.61770000000000003</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="J8">
-        <v>0.33550000000000002</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="K8">
-        <v>0.49280000000000002</v>
+        <v>4.9299999999999997E-2</v>
       </c>
       <c r="L8">
-        <v>2.0291000000000001</v>
+        <v>5.4699999999999999E-2</v>
       </c>
       <c r="M8">
-        <v>0.45169999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="N8">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="O8">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="P8">
+        <v>2.98E-2</v>
+      </c>
+      <c r="Q8">
+        <v>2.7099999999999999E-2</v>
+      </c>
+      <c r="R8">
+        <v>2.46E-2</v>
+      </c>
+      <c r="S8">
+        <v>1.32E-2</v>
+      </c>
+      <c r="T8">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="U8">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="V8">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="W8">
+        <v>4.5199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>0.42959999999999998</v>
       </c>
       <c r="C9">
-        <v>0.48620000000000002</v>
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="D9">
-        <v>0.88</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E9">
-        <v>0.4022</v>
+        <v>4.02E-2</v>
       </c>
       <c r="F9">
-        <v>0.58160000000000001</v>
+        <v>5.8200000000000002E-2</v>
       </c>
       <c r="G9">
         <v>0.15379999999999999</v>
       </c>
       <c r="H9">
-        <v>0.61770000000000003</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.24890000000000001</v>
+        <v>2.4899999999999999E-2</v>
       </c>
       <c r="K9">
-        <v>0.22739999999999999</v>
+        <v>2.2700000000000001E-2</v>
       </c>
       <c r="L9">
-        <v>0.77210000000000001</v>
+        <v>2.0500000000000001E-2</v>
       </c>
       <c r="M9">
-        <v>0.1072</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>1.78E-2</v>
+      </c>
+      <c r="N9">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="O9">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="P9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="Q9">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="R9">
+        <v>1.26E-2</v>
+      </c>
+      <c r="S9">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="T9">
+        <v>4.6699999999999998E-2</v>
+      </c>
+      <c r="U9">
+        <v>1.09E-2</v>
+      </c>
+      <c r="V9">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="W9">
+        <v>1.0699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>0.13100000000000001</v>
       </c>
       <c r="C10">
-        <v>0.46910000000000002</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="D10">
-        <v>0.44319999999999998</v>
+        <v>4.4299999999999999E-2</v>
       </c>
       <c r="E10">
-        <v>0.37130000000000002</v>
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="F10">
-        <v>0.43330000000000002</v>
+        <v>4.3299999999999998E-2</v>
       </c>
       <c r="G10">
         <v>3.3300000000000003E-2</v>
       </c>
       <c r="H10">
-        <v>0.33550000000000002</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="I10">
-        <v>0.24890000000000001</v>
+        <v>2.4899999999999999E-2</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.15409999999999999</v>
+        <v>1.54E-2</v>
       </c>
       <c r="L10">
-        <v>0.37909999999999999</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="M10">
-        <v>5.0500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="N10">
+        <v>1.01E-2</v>
+      </c>
+      <c r="O10">
+        <v>1.01E-2</v>
+      </c>
+      <c r="P10">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="Q10">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="R10">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="S10">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="T10">
+        <v>1.18E-2</v>
+      </c>
+      <c r="U10">
+        <v>1.32E-2</v>
+      </c>
+      <c r="V10">
+        <v>3.8E-3</v>
+      </c>
+      <c r="W10">
+        <v>5.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>0.188</v>
       </c>
       <c r="C11">
-        <v>0.71719999999999995</v>
+        <v>7.17E-2</v>
       </c>
       <c r="D11">
-        <v>1.5625</v>
+        <v>0.15629999999999999</v>
       </c>
       <c r="E11">
-        <v>0.78459999999999996</v>
+        <v>7.85E-2</v>
       </c>
       <c r="F11">
-        <v>2.5154000000000001</v>
+        <v>0.2515</v>
       </c>
       <c r="G11">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="H11">
-        <v>0.49280000000000002</v>
+        <v>4.9299999999999997E-2</v>
       </c>
       <c r="I11">
-        <v>0.22739999999999999</v>
+        <v>2.2700000000000001E-2</v>
       </c>
       <c r="J11">
-        <v>0.15409999999999999</v>
+        <v>1.54E-2</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1.0865</v>
+        <v>4.2599999999999999E-2</v>
       </c>
       <c r="M11">
-        <v>5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="N11">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="O11">
+        <v>1.47E-2</v>
+      </c>
+      <c r="P11">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="Q11">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="R11">
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="S11">
+        <v>1.23E-2</v>
+      </c>
+      <c r="T11">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="U11">
+        <v>1.54E-2</v>
+      </c>
+      <c r="V11">
+        <v>1.09E-2</v>
+      </c>
+      <c r="W11">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B12">
+        <v>0.16270000000000001</v>
+      </c>
+      <c r="C12">
+        <v>6.1699999999999998E-2</v>
+      </c>
+      <c r="D12">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="E12">
+        <v>6.7299999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G12">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="H12">
+        <v>5.4699999999999999E-2</v>
+      </c>
+      <c r="I12">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="J12">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="K12">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="N12">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="O12">
+        <v>1.15E-2</v>
+      </c>
+      <c r="P12">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="Q12">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="R12">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="S12">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="T12">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="U12">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="V12">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="W12">
+        <v>6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="C13">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="D13">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="E13">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="F13">
+        <v>1.4197</v>
+      </c>
+      <c r="G13">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="H13">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="I13">
+        <v>1.78E-2</v>
+      </c>
+      <c r="J13">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="K13">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="L13">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="O13">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="P13">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="Q13">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="R13">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="S13">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="T13">
+        <v>1.14E-2</v>
+      </c>
+      <c r="U13">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="V13">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="W13">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.1047</v>
+      </c>
+      <c r="C14">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="D14">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="E14">
+        <v>7.1900000000000006E-2</v>
+      </c>
+      <c r="F14">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="G14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H14">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="I14">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="J14">
+        <v>1.01E-2</v>
+      </c>
+      <c r="K14">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="L14">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="M14">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>8.6E-3</v>
+      </c>
+      <c r="P14">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="Q14">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="R14">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="S14">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="T14">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="U14">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="V14">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="W14">
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0.35830000000000001</v>
+      </c>
+      <c r="C15">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D15">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="E15">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.14810000000000001</v>
+      </c>
+      <c r="H15">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="I15">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="J15">
+        <v>1.01E-2</v>
+      </c>
+      <c r="K15">
+        <v>1.47E-2</v>
+      </c>
+      <c r="L15">
+        <v>1.15E-2</v>
+      </c>
+      <c r="M15">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="N15">
+        <v>8.6E-3</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="Q15">
+        <v>1.01E-2</v>
+      </c>
+      <c r="R15">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="S15">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="T15">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="U15">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="V15">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="W15">
+        <v>5.3E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0.1062</v>
+      </c>
+      <c r="C16">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="D16">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="E16">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.1638</v>
+      </c>
+      <c r="G16">
+        <v>2.47E-2</v>
+      </c>
+      <c r="H16">
+        <v>2.98E-2</v>
+      </c>
+      <c r="I16">
+        <v>1.4E-2</v>
+      </c>
+      <c r="J16">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="K16">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="L16">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="M16">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N16">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="O16">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="R16">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="S16">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="T16">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="U16">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="V16">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="W16">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0.13170000000000001</v>
+      </c>
+      <c r="C17">
+        <v>2.35E-2</v>
+      </c>
+      <c r="D17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E17">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="F17">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="G17">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="H17">
+        <v>2.7099999999999999E-2</v>
+      </c>
+      <c r="I17">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J17">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="K17">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="L17">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="M17">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="N17">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="O17">
+        <v>1.01E-2</v>
+      </c>
+      <c r="P17">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="S17">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="T17">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="U17">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="V17">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="W17">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>9.5200000000000007E-2</v>
+      </c>
+      <c r="C18">
+        <v>5.8299999999999998E-2</v>
+      </c>
+      <c r="D18">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E18">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.1057</v>
+      </c>
+      <c r="G18">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="H18">
+        <v>2.46E-2</v>
+      </c>
+      <c r="I18">
+        <v>1.26E-2</v>
+      </c>
+      <c r="J18">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="K18">
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="L18">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="M18">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="N18">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="O18">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="P18">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="Q18">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0.01</v>
+      </c>
+      <c r="T18">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="U18">
+        <v>1.11E-2</v>
+      </c>
+      <c r="V18">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="W18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="C19">
+        <v>1.5952999999999999</v>
+      </c>
+      <c r="D19">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="E19">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="F19">
+        <v>3.09E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.34E-2</v>
+      </c>
+      <c r="H19">
+        <v>1.32E-2</v>
+      </c>
+      <c r="I19">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="J19">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="K19">
+        <v>1.23E-2</v>
+      </c>
+      <c r="L19">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="M19">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="N19">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="O19">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="P19">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="Q19">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="R19">
+        <v>0.01</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="U19">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="V19">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="W19">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>0.86829999999999996</v>
+      </c>
+      <c r="C20">
+        <v>2.58E-2</v>
+      </c>
+      <c r="D20">
+        <v>5.9799999999999999E-2</v>
+      </c>
+      <c r="E20">
+        <v>2.24E-2</v>
+      </c>
+      <c r="F20">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="G20">
+        <v>0.19339999999999999</v>
+      </c>
+      <c r="H20">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="I20">
+        <v>4.6699999999999998E-2</v>
+      </c>
+      <c r="J20">
+        <v>1.18E-2</v>
+      </c>
+      <c r="K20">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="L20">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M20">
+        <v>1.14E-2</v>
+      </c>
+      <c r="N20">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="O20">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="P20">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="Q20">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="R20">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="S20">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="V20">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="W20">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="C21">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="D21">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="E21">
+        <v>6.0100000000000001E-2</v>
+      </c>
+      <c r="F21">
+        <v>4.7199999999999999E-2</v>
+      </c>
+      <c r="G21">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="H21">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="I21">
+        <v>1.09E-2</v>
+      </c>
+      <c r="J21">
+        <v>1.32E-2</v>
+      </c>
+      <c r="K21">
+        <v>1.54E-2</v>
+      </c>
+      <c r="L21">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="M21">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="N21">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="O21">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="P21">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="Q21">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="R21">
+        <v>1.11E-2</v>
+      </c>
+      <c r="S21">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="T21">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="W21">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
         <v>9.1600000000000001E-2</v>
       </c>
-      <c r="C12">
-        <v>0.11890000000000001</v>
-      </c>
-      <c r="D12">
-        <v>0.58460000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.1119</v>
-      </c>
-      <c r="F12">
-        <v>0.25619999999999998</v>
-      </c>
-      <c r="G12">
+      <c r="C22">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="D22">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="E22">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F22">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="G22">
         <v>1.8200000000000001E-2</v>
       </c>
-      <c r="H12">
-        <v>0.2029</v>
-      </c>
-      <c r="I12">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="J12">
-        <v>3.7900000000000003E-2</v>
-      </c>
-      <c r="K12">
-        <v>0.1087</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
+      <c r="H22">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="I22">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="J22">
+        <v>3.8E-3</v>
+      </c>
+      <c r="K22">
+        <v>1.09E-2</v>
+      </c>
+      <c r="L22">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="M22">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="N22">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="O22">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="P22">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="Q22">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="R22">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="S22">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="T22">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="U22">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
         <v>0.11210000000000001</v>
       </c>
-      <c r="C13">
-        <v>0.1004</v>
-      </c>
-      <c r="D13">
-        <v>0.19639999999999999</v>
-      </c>
-      <c r="E13">
-        <v>8.9599999999999999E-2</v>
-      </c>
-      <c r="F13">
-        <v>0.1615</v>
-      </c>
-      <c r="G13">
+      <c r="C23">
+        <v>0.01</v>
+      </c>
+      <c r="D23">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="E23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F23">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="G23">
         <v>2.1399999999999999E-2</v>
       </c>
-      <c r="H13">
-        <v>0.45169999999999999</v>
-      </c>
-      <c r="I13">
-        <v>0.1072</v>
-      </c>
-      <c r="J13">
-        <v>5.0500000000000003E-2</v>
-      </c>
-      <c r="K13">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="L13">
-        <v>0.2195</v>
-      </c>
-      <c r="M13">
+      <c r="H23">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="I23">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="J23">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="K23">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="L23">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="M23">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="N23">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="O23">
+        <v>5.3E-3</v>
+      </c>
+      <c r="P23">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="Q23">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="R23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="S23">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="T23">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="U23">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="V23">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="W23">
         <v>0</v>
       </c>
     </row>

</xml_diff>